<commit_message>
Cambios en escenarios de calidad
</commit_message>
<xml_diff>
--- a/ExtraClase/FuncionalidadesCriticas.xlsx
+++ b/ExtraClase/FuncionalidadesCriticas.xlsx
@@ -5,20 +5,31 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4a956f53eadd4fd8/Escritorio/U/2024-2/IS2/ExtraClase/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arias Ramirez\OneDrive\Escritorio\U\2024-2\IS2\ExtraClase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_AD4D2F04E46CFB4ACB3E202A4556F4B4693EDF10" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C59D768-CEDF-49DD-BEBB-EEA4956D9E0E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4512C2-6E94-41F5-8841-4ACEA989926D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FuncionalidadesCriticas " sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -119,15 +130,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,19 +152,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,7 +468,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,13 +483,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -462,13 +497,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -476,35 +511,51 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="C3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -512,18 +563,20 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="1" t="s">

</xml_diff>